<commit_message>
CFWH and OFWH Efficiencies
</commit_message>
<xml_diff>
--- a/me312/ME312_W16_project_specification.xlsx
+++ b/me312/ME312_W16_project_specification.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="45">
   <si>
     <t>Team Name</t>
   </si>
@@ -1552,8 +1552,8 @@
   </sheetPr>
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1802,7 +1802,9 @@
       <c r="B28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D28" s="0" t="s">
         <v>10</v>
       </c>
@@ -1820,7 +1822,9 @@
       <c r="B30" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D30" s="0" t="s">
         <v>10</v>
       </c>
@@ -1840,7 +1844,9 @@
       <c r="B33" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1" t="n">
+        <v>7.6</v>
+      </c>
       <c r="D33" s="0" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +1855,9 @@
       <c r="B34" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1" t="n">
+        <v>22.6</v>
+      </c>
       <c r="D34" s="0" t="s">
         <v>10</v>
       </c>
@@ -1858,7 +1866,9 @@
       <c r="B35" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="n">
+        <v>37.3</v>
+      </c>
       <c r="D35" s="0" t="s">
         <v>10</v>
       </c>
@@ -1867,7 +1877,9 @@
       <c r="B36" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="n">
+        <v>69.3</v>
+      </c>
       <c r="D36" s="0" t="s">
         <v>10</v>
       </c>
@@ -1882,7 +1894,9 @@
       <c r="B38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="1" t="n">
+        <v>3.8</v>
+      </c>
       <c r="D38" s="0" t="s">
         <v>10</v>
       </c>
@@ -1891,7 +1905,9 @@
       <c r="B39" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="1"/>
+      <c r="C39" s="1" t="n">
+        <v>5.5</v>
+      </c>
       <c r="D39" s="0" t="s">
         <v>10</v>
       </c>
@@ -1900,7 +1916,9 @@
       <c r="B40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" s="1" t="n">
+        <v>90.5</v>
+      </c>
       <c r="D40" s="0" t="s">
         <v>10</v>
       </c>
@@ -1909,7 +1927,9 @@
       <c r="B41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D41" s="0" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1938,9 @@
       <c r="B42" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="1" t="n">
+        <v>95.4</v>
+      </c>
       <c r="D42" s="0" t="s">
         <v>10</v>
       </c>
@@ -1927,13 +1949,20 @@
       <c r="B43" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="1"/>
+      <c r="C43" s="1" t="n">
+        <v>96.6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D44" s="0" t="s">
         <v>10</v>
       </c>

</xml_diff>